<commit_message>
fix: resolve TS errors and Node engine mismatch in frontend build
</commit_message>
<xml_diff>
--- a/Karşıyaka Ürün Envanteri.xlsx
+++ b/Karşıyaka Ürün Envanteri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\acursor\jul4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770A45E3-C647-43AC-B662-9EE957B711C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7457CCC8-FCC6-4164-BD5C-3F08D6B46CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{759D3DE3-FA60-4AE3-85DA-DE3761852ED1}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{759D3DE3-FA60-4AE3-85DA-DE3761852ED1}"/>
   </bookViews>
   <sheets>
     <sheet name="BB" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CLP  '!$A$1:$G$24</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1072,13 +1061,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,20 +1403,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B59C2E-925E-4CF4-95F8-C480249EA179}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1474,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1497,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1520,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1543,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1589,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1612,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1635,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1658,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1681,7 +1669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1704,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1750,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -1773,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1796,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -1819,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1842,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1865,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -1888,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -1911,7 +1899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -1957,7 +1945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1980,7 +1968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
@@ -2003,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
@@ -2026,7 +2014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
@@ -2049,7 +2037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -2072,7 +2060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
@@ -2095,7 +2083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -2118,7 +2106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
@@ -2141,7 +2129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
@@ -2164,7 +2152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -2187,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
@@ -2210,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>78</v>
       </c>
@@ -2233,7 +2221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>78</v>
       </c>
@@ -2256,7 +2244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>82</v>
       </c>
@@ -2279,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
@@ -2302,7 +2290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>86</v>
       </c>
@@ -2325,7 +2313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>86</v>
       </c>
@@ -2348,7 +2336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>90</v>
       </c>
@@ -2371,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
@@ -2394,7 +2382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2417,7 +2405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>54</v>
       </c>
@@ -2440,7 +2428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
@@ -2463,7 +2451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>96</v>
       </c>
@@ -2486,7 +2474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>96</v>
       </c>
@@ -2509,7 +2497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
@@ -2532,7 +2520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>18</v>
       </c>
@@ -2555,7 +2543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>102</v>
       </c>
@@ -2578,7 +2566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>102</v>
       </c>
@@ -2601,7 +2589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>65</v>
       </c>
@@ -2624,7 +2612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>65</v>
       </c>
@@ -2647,7 +2635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>31</v>
       </c>
@@ -2670,7 +2658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>31</v>
       </c>
@@ -2693,7 +2681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>74</v>
       </c>
@@ -2716,7 +2704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>74</v>
       </c>
@@ -2739,7 +2727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
@@ -2762,7 +2750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>113</v>
       </c>
@@ -2785,7 +2773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>40</v>
       </c>
@@ -2808,7 +2796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>40</v>
       </c>
@@ -2831,7 +2819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>82</v>
       </c>
@@ -2854,7 +2842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>82</v>
       </c>
@@ -2877,7 +2865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +2888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -2923,7 +2911,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>96</v>
       </c>
@@ -2946,7 +2934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>18</v>
       </c>
@@ -2969,7 +2957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>18</v>
       </c>
@@ -2992,7 +2980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>125</v>
       </c>
@@ -3015,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
@@ -3038,7 +3026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>27</v>
       </c>
@@ -3061,7 +3049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
@@ -3084,7 +3072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>31</v>
       </c>
@@ -3107,7 +3095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>31</v>
       </c>
@@ -3130,7 +3118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>35</v>
       </c>
@@ -3153,7 +3141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>35</v>
       </c>
@@ -3176,7 +3164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>113</v>
       </c>
@@ -3199,7 +3187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>113</v>
       </c>
@@ -3222,7 +3210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -3245,7 +3233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>78</v>
       </c>
@@ -3268,7 +3256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>139</v>
       </c>
@@ -3291,7 +3279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>139</v>
       </c>
@@ -3314,7 +3302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>179</v>
       </c>
@@ -3337,7 +3325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>179</v>
       </c>
@@ -3360,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>0</v>
       </c>
@@ -3383,7 +3371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>7</v>
       </c>
@@ -3406,7 +3394,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>7</v>
       </c>
@@ -3429,7 +3417,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>151</v>
       </c>
@@ -3452,7 +3440,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>151</v>
       </c>
@@ -3475,7 +3463,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>156</v>
       </c>
@@ -3498,7 +3486,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>22</v>
       </c>
@@ -3521,7 +3509,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>27</v>
       </c>
@@ -3544,7 +3532,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>74</v>
       </c>
@@ -3567,7 +3555,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>162</v>
       </c>
@@ -3590,7 +3578,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>162</v>
       </c>
@@ -3613,7 +3601,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>166</v>
       </c>
@@ -3636,7 +3624,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>169</v>
       </c>
@@ -3659,7 +3647,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>178</v>
       </c>
@@ -3682,7 +3670,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>179</v>
       </c>
@@ -3705,7 +3693,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>180</v>
       </c>
@@ -3738,20 +3726,20 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3774,7 +3762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>182</v>
       </c>
@@ -3797,7 +3785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -3820,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
@@ -3843,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>196</v>
       </c>
@@ -3866,7 +3854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>200</v>
       </c>
@@ -3889,7 +3877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>204</v>
       </c>
@@ -3912,7 +3900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>208</v>
       </c>
@@ -3935,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>213</v>
       </c>
@@ -3958,7 +3946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>216</v>
       </c>
@@ -3981,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>221</v>
       </c>
@@ -4004,7 +3992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>225</v>
       </c>
@@ -4027,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -4050,7 +4038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>182</v>
       </c>
@@ -4073,7 +4061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>188</v>
       </c>
@@ -4096,7 +4084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>192</v>
       </c>
@@ -4119,7 +4107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>196</v>
       </c>
@@ -4142,7 +4130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>200</v>
       </c>
@@ -4165,7 +4153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>204</v>
       </c>
@@ -4188,7 +4176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>208</v>
       </c>
@@ -4211,7 +4199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>213</v>
       </c>
@@ -4234,7 +4222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>216</v>
       </c>
@@ -4257,7 +4245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>221</v>
       </c>
@@ -4280,7 +4268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>225</v>
       </c>
@@ -4313,19 +4301,19 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4348,7 +4336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>226</v>
       </c>
@@ -4371,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>226</v>
       </c>
@@ -4404,19 +4392,19 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4439,7 +4427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>315</v>
       </c>
@@ -4462,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>316</v>
       </c>
@@ -4495,20 +4483,20 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4531,7 +4519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>230</v>
       </c>
@@ -4554,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>235</v>
       </c>
@@ -4577,7 +4565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>240</v>
       </c>
@@ -4600,7 +4588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>244</v>
       </c>
@@ -4623,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>247</v>
       </c>
@@ -4646,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>250</v>
       </c>
@@ -4669,7 +4657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>253</v>
       </c>
@@ -4692,7 +4680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>239</v>
       </c>
@@ -4715,14 +4703,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>256</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -4731,10 +4719,10 @@
       <c r="E10" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>9</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -4748,19 +4736,19 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4783,7 +4771,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>271</v>
       </c>
@@ -4806,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>272</v>
       </c>
@@ -4829,7 +4817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>273</v>
       </c>
@@ -4852,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>274</v>
       </c>
@@ -4875,7 +4863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>275</v>
       </c>
@@ -4898,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>276</v>
       </c>
@@ -4921,7 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>277</v>
       </c>
@@ -4957,17 +4945,17 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4990,7 +4978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>280</v>
       </c>
@@ -5013,7 +5001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>283</v>
       </c>
@@ -5036,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>286</v>
       </c>
@@ -5059,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>289</v>
       </c>
@@ -5082,7 +5070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>292</v>
       </c>
@@ -5105,14 +5093,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>295</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -5128,14 +5116,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>298</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -5151,14 +5139,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>301</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -5174,14 +5162,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>304</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>170</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -5197,14 +5185,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>307</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>209</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -5220,14 +5208,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>310</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">

</xml_diff>